<commit_message>
Corrections erreurs 6, 7, 13, 16
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_equipe.xlsx
+++ b/Fichiers equipe/revue_code_equipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinaa\Documents\Maintenace Logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29A390E-184D-46E4-994A-AB9592EA7626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BD5064-F195-48C8-A606-979572E3CD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -110,8 +110,65 @@
     <t>en cours</t>
   </si>
   <si>
+    <t>Elie,Khalil</t>
+  </si>
+  <si>
+    <t>Elie, Khalil</t>
+  </si>
+  <si>
+    <t>Défaut + Amélioration</t>
+  </si>
+  <si>
+    <t>Défaut + Cosmétique</t>
+  </si>
+  <si>
+    <t>Cosmétique + Amélioration</t>
+  </si>
+  <si>
+    <t>45-50-57-59 etc</t>
+  </si>
+  <si>
+    <t>Défaut</t>
+  </si>
+  <si>
+    <t>Cosmétique</t>
+  </si>
+  <si>
+    <t>Défaut + Erreur</t>
+  </si>
+  <si>
+    <t>162 + 165</t>
+  </si>
+  <si>
+    <t>Amélioration + Cosmétique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amélioration + Cosmétique </t>
+  </si>
+  <si>
+    <t>Erreur</t>
+  </si>
+  <si>
+    <t>Elie</t>
+  </si>
+  <si>
+    <t>fait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amélioration +Cosmétique </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>dina, Elie, Khalil</t>
+  </si>
+  <si>
+    <t>Dina</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">if __name__ == '__main__': programme_principal()  /   Il n'ya pas de main dans l'application </t>
+      <t>Lignes vierges ne sont pas toujours respectés entre les partie du code pour la lisibilité</t>
     </r>
     <r>
       <rPr>
@@ -121,77 +178,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(monsieur_tartempion.py)</t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
-    <t>Elie,Khalil</t>
-  </si>
-  <si>
-    <t>Elie, Khalil</t>
-  </si>
-  <si>
-    <t>Défaut + Amélioration</t>
-  </si>
-  <si>
-    <t>Défaut + Cosmétique</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">les noms des fonctions  (splacher et splasher)  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>Cosmétique + Amélioration</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Des lignes trop longues dépassant 80 caractères(selon PEP8). </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>45-50-57-59 etc</t>
-  </si>
-  <si>
-    <r>
-      <t>"title": variable non utilisé.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>Défaut</t>
-  </si>
-  <si>
-    <t>Cosmétique</t>
+    <t xml:space="preserve">Manque de commentaire dans le code  </t>
+  </si>
+  <si>
+    <t>Laisser une ligne vide à la fin du code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La variable (temps_actuel, musique_questions_controles) est utilisé avant de l'assigner une valeurs  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction(programme_principal()) est très longue , il faut séparer les fonctionnalité en plusieurs fonctions plus significatifs et lisibles . </t>
+  </si>
+  <si>
+    <t>"title": variable non utilisé.</t>
   </si>
   <si>
     <r>
@@ -205,129 +208,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
+      <t xml:space="preserve"> </t>
     </r>
   </si>
   <si>
-    <t>78 + 114 + 124</t>
-  </si>
-  <si>
-    <t>Noms de variables non significatifs (ex: "banque"ce sera mieux si on le nomme "liste_questions")</t>
+    <t>Des lignes trop longues dépassant 80 caractères(selon PEP8).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les noms des fonctions  (splacher et splasher)  </t>
+  </si>
+  <si>
+    <t>if __name__ == '__main__': programme_principal()  /   Il n'ya pas de main dans l'application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La variable (TEMPS_EPREUVE) n'a jamais été déclarée ou initialisée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la paramètre "pardessus: bool" n'est pas necessaire , il est utilisé une seul fois et c'est exactement le même code dans l'autre méthode d'affichage  </t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">la fonction(programme_principal()) est très longue , il faut séparer les fonctionnalité en plusieurs fonctions plus significatifs et lisibles . </t>
+      <t xml:space="preserve">Questions No.251 est une question de (*)    "251	 *       Mauvaise  	 Question ".   </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>Défaut + Erreur</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">La variable (temps_actuel, musique_questions_controles) est utilisé avant de l'assigner une valeurs  </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>162 + 165</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Laisser une ligne vide à la fin du code </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>Amélioration + Cosmétique</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Manque de commentaire dans le code  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Lignes vierges ne sont pas toujours respectés entre les partie du code pour la lisibilité</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Amélioration + Cosmétique </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">La variable (TEMPS_EPREUVE) n'a jamais été déclarée ou initialisée </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t>Erreur</t>
-  </si>
-  <si>
-    <t>Elie</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Questions No.251 est une question de (*)    "251	 *       Mauvaise  	 Question ".    </t>
-    </r>
-    <r>
-      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -338,56 +254,29 @@
     </r>
   </si>
   <si>
-    <t>fait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amélioration +Cosmétique </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">la paramètre "pardessus: bool" n'est pas necessaire , il est utilisé une seul fois et c'est exactement le même code dans l'autre méthode d'affichage  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Duplication du code dans trois fonctions : afficher , effacer_question ,effacer_question_affichee, splasher_equipe , splacher_titre</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(monsieur_tartempion.py)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>dina</t>
-  </si>
-  <si>
-    <t>dina, Elie, Khalil</t>
+    <t>Noms de variables non significatifs (banque, nombre)</t>
+  </si>
+  <si>
+    <t>Elie,Khalil,Dina</t>
+  </si>
+  <si>
+    <t>Duplication du code dans trois fonctions : afficher , effacer_question, splasher_equipe , splacher_titre</t>
+  </si>
+  <si>
+    <t>79 + 124</t>
+  </si>
+  <si>
+    <t>78 + 114</t>
+  </si>
+  <si>
+    <t>Les fonctions effacer_question et effacer_question_affichee ont exactement la même fonctionnalité</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,6 +309,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -532,11 +437,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,15 +776,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17.850000000000001" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
@@ -914,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -975,14 +880,14 @@
         <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>23</v>
@@ -996,17 +901,17 @@
         <v>22</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1014,19 +919,19 @@
         <v>3</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>23</v>
@@ -1040,17 +945,17 @@
         <v>45</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="11" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1061,64 +966,60 @@
         <v>55</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
         <v>6</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="B17" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="15"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="10">
         <v>7</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="11">
         <v>95</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="34.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1129,35 +1030,35 @@
         <v>128</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>9</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>23</v>
@@ -1171,14 +1072,14 @@
         <v>241</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>23</v>
@@ -1192,16 +1093,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>23</v>
@@ -1215,40 +1116,38 @@
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="10">
         <v>13</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="10">
         <v>205</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>23</v>
+      <c r="C24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1259,17 +1158,17 @@
         <v>251</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1280,30 +1179,38 @@
         <v>48</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>54</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="13">
         <v>16</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="8" t="s">
-        <v>23</v>
+      <c r="B27" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
corriger les erreur de revue de code de l'équipe :  5, 9, 12, 17
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_equipe.xlsx
+++ b/Fichiers equipe/revue_code_equipe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinaa\Documents\Maintenace Logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khalil\Desktop\BdeB\CETTE SESSION\Cours_maintenance\TP1\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BD5064-F195-48C8-A606-979572E3CD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71594E-5BFF-4935-A4E4-AC4A1C6E29A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -108,9 +97,6 @@
   </si>
   <si>
     <t>en cours</t>
-  </si>
-  <si>
-    <t>Elie,Khalil</t>
   </si>
   <si>
     <t>Elie, Khalil</t>
@@ -271,12 +257,65 @@
   <si>
     <t>Les fonctions effacer_question et effacer_question_affichee ont exactement la même fonctionnalité</t>
   </si>
+  <si>
+    <t>Khalil</t>
+  </si>
+  <si>
+    <t>défaut</t>
+  </si>
+  <si>
+    <r>
+      <t>indicateurs =</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[gui.Image(data=indicateur_vide_base64(), key=f'INDICATEUR-{i}', pad=(4, 10)) for i in range(NB_QUESTIONS)]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ des ajouts de plus qui font rien </t>
+    </r>
+  </si>
+  <si>
+    <t>khalil</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,8 +370,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,8 +408,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -398,11 +449,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -441,6 +514,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -760,18 +852,18 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.09765625" customWidth="1"/>
-    <col min="3" max="3" width="25.69921875" customWidth="1"/>
-    <col min="4" max="4" width="98.09765625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="98.109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="20.296875" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,7 +911,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -872,7 +964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>1</v>
       </c>
@@ -880,14 +972,14 @@
         <v>21</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>23</v>
@@ -901,17 +993,17 @@
         <v>22</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -919,25 +1011,25 @@
         <v>3</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.3" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>4</v>
       </c>
@@ -945,38 +1037,38 @@
         <v>45</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="16">
         <v>5</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="17">
         <v>55</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>23</v>
+      <c r="C16" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -984,17 +1076,17 @@
         <v>6</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>23</v>
@@ -1009,20 +1101,20 @@
         <v>95</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="34.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="34.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>8</v>
       </c>
@@ -1030,38 +1122,38 @@
         <v>128</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="16">
         <v>9</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>23</v>
+      <c r="C20" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1072,14 +1164,14 @@
         <v>241</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>23</v>
@@ -1093,40 +1185,40 @@
         <v>21</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="16">
         <v>12</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>23</v>
+      <c r="C23" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1137,17 +1229,17 @@
         <v>205</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1158,17 +1250,17 @@
         <v>251</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1179,17 +1271,17 @@
         <v>48</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1197,33 +1289,41 @@
         <v>16</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
         <v>17</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="8" t="s">
-        <v>23</v>
+      <c r="B28" s="19">
+        <v>77</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Rajouter mon nom qui a été effacé sur une des tâche fait en 2
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_equipe.xlsx
+++ b/Fichiers equipe/revue_code_equipe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khalil\Desktop\BdeB\CETTE SESSION\Cours_maintenance\TP1\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D71594E-5BFF-4935-A4E4-AC4A1C6E29A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD31DAC-21D2-4D38-8B90-8FAC5DF8AF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>FICHE DE REVUE DE CODE</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>khalil</t>
+  </si>
+  <si>
+    <t>Elie, Dina</t>
   </si>
 </sst>
 </file>
@@ -446,17 +449,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -471,11 +463,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -510,30 +515,40 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,34 +866,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="98.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="98.140625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.850000000000001" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -892,7 +907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
@@ -906,7 +921,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -920,20 +935,20 @@
         <v>45209</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
@@ -941,7 +956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -964,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1</v>
       </c>
@@ -982,10 +997,10 @@
         <v>36</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>2</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>3</v>
       </c>
@@ -1026,10 +1041,10 @@
         <v>36</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>4</v>
       </c>
@@ -1050,28 +1065,29 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
         <v>5</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="15">
         <v>55</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>6</v>
       </c>
@@ -1086,14 +1102,14 @@
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>7</v>
       </c>
@@ -1110,11 +1126,12 @@
       <c r="F18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="34.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="1:8" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>8</v>
       </c>
@@ -1135,28 +1152,28 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="16">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
         <v>9</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>10</v>
       </c>
@@ -1177,7 +1194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>11</v>
       </c>
@@ -1200,28 +1217,28 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
         <v>12</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17" t="s">
+      <c r="E23" s="14"/>
+      <c r="F23" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>13</v>
       </c>
@@ -1242,7 +1259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>14</v>
       </c>
@@ -1263,7 +1280,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>15</v>
       </c>
@@ -1284,7 +1301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>16</v>
       </c>
@@ -1305,28 +1322,28 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="16">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
         <v>17</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="17">
         <v>77</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>18</v>
       </c>
@@ -1339,7 +1356,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>19</v>
       </c>
@@ -1352,7 +1369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>20</v>
       </c>
@@ -1363,7 +1380,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>21</v>
       </c>
@@ -1374,7 +1391,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>22</v>
       </c>
@@ -1385,7 +1402,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>23</v>
       </c>
@@ -1396,7 +1413,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>24</v>
       </c>
@@ -1407,7 +1424,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
developper la nouvelle fonctionnalité
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_equipe.xlsx
+++ b/Fichiers equipe/revue_code_equipe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efrie\OneDrive - Collège de Bois-de-Boulogne\genie logiciel\Session 5 - Automne 2023\Maintenance logiciel\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591F5315-AA21-438A-B5B9-2BCC6B65C6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67289C5C-6B18-4853-8D01-122078F4DB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -910,11 +910,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Ajoute d'un nouveau test qui verifie la changement de la question
</commit_message>
<xml_diff>
--- a/Fichiers equipe/revue_code_equipe.xlsx
+++ b/Fichiers equipe/revue_code_equipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lion0203\projets\5GP-Travail_pratique_1\Fichiers equipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE893E39-2D01-4FDF-8639-6156CBE14A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E0C236-DD69-4CD2-9EC0-2330DCE46017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H28" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,7 +972,9 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>45224</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -1350,7 +1352,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18">
+      <c r="A28" s="9">
         <v>17</v>
       </c>
       <c r="B28" s="12">
@@ -1363,11 +1365,11 @@
         <v>56</v>
       </c>
       <c r="E28" s="12"/>
-      <c r="F28" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>23</v>
+      <c r="F28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>